<commit_message>
updating program to a newer version
</commit_message>
<xml_diff>
--- a/exam_document/answer_key.xlsx
+++ b/exam_document/answer_key.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>B_TF</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>A_MC</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>B_MC</t>
         </is>
       </c>
     </row>
@@ -463,39 +453,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -507,39 +477,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>B</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>D</t>
         </is>
       </c>
     </row>
@@ -550,16 +500,6 @@
         </is>
       </c>
       <c r="B6" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
         <is>
           <t>D</t>
         </is>

</xml_diff>